<commit_message>
changed the template name to WATR
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19487DC-2281-433B-8F8A-0276867F0AAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082255DB-1BF0-4B82-8660-CB66193C26F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -3706,121 +3706,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3863,6 +3764,105 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4703,7 +4703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFC53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -5221,7 +5221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AF9770-A07B-4681-91C3-E6CA1B6C7937}">
   <dimension ref="A1:IR30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -6753,10 +6753,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="125">
-        <f>(28)/38*100</f>
-        <v>73.68421052631578</v>
-      </c>
+      <c r="A29" s="125"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="126" t="s">
@@ -6781,8 +6778,8 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6807,16 +6804,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="185" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="179"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="186"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6830,13 +6827,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="182"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="190"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6848,13 +6845,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="197"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6866,12 +6863,12 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="180" t="s">
+      <c r="A4" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="180"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6884,13 +6881,13 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="164"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="214"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6902,13 +6899,13 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="162"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="166"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="164"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6920,13 +6917,13 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="165" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="164"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6938,13 +6935,13 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="165" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="162"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="164"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6956,16 +6953,16 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="193" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="185"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6975,16 +6972,16 @@
       <c r="Q9" s="99"/>
     </row>
     <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="186" t="s">
+      <c r="A10" s="195" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="187"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="187"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="188"/>
+      <c r="B10" s="196"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="197"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6994,10 +6991,10 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="200" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="194"/>
+      <c r="B11" s="201"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -7007,10 +7004,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="189" t="s">
+      <c r="F11" s="199" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="189"/>
+      <c r="G11" s="199"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -7022,18 +7019,18 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="172" t="s">
+      <c r="A12" s="191" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="183"/>
-      <c r="C12" s="190" t="s">
+      <c r="B12" s="192"/>
+      <c r="C12" s="182" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="191"/>
-      <c r="E12" s="191"/>
-      <c r="F12" s="191"/>
-      <c r="G12" s="191"/>
-      <c r="H12" s="192"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="183"/>
+      <c r="G12" s="183"/>
+      <c r="H12" s="184"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -7486,14 +7483,14 @@
       <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="176" t="s">
+      <c r="A27" s="187" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="177"/>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7510,18 +7507,18 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="172" t="s">
+      <c r="A28" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="190" t="s">
+      <c r="B28" s="198"/>
+      <c r="C28" s="182" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="191"/>
-      <c r="E28" s="191"/>
-      <c r="F28" s="191"/>
-      <c r="G28" s="191"/>
-      <c r="H28" s="192"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="183"/>
+      <c r="F28" s="183"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="184"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7899,14 +7896,14 @@
       <c r="Q40" s="93"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="176" t="s">
+      <c r="A41" s="187" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
-      <c r="D41" s="177"/>
-      <c r="E41" s="177"/>
-      <c r="F41" s="177"/>
+      <c r="B41" s="188"/>
+      <c r="C41" s="188"/>
+      <c r="D41" s="188"/>
+      <c r="E41" s="188"/>
+      <c r="F41" s="188"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7923,18 +7920,18 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="172" t="s">
+      <c r="A42" s="191" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="173"/>
-      <c r="C42" s="190" t="s">
+      <c r="B42" s="198"/>
+      <c r="C42" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="191"/>
-      <c r="E42" s="191"/>
-      <c r="F42" s="191"/>
-      <c r="G42" s="191"/>
-      <c r="H42" s="192"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="183"/>
+      <c r="G42" s="183"/>
+      <c r="H42" s="184"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -8253,14 +8250,14 @@
       <c r="Q52" s="93"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="176" t="s">
+      <c r="A53" s="187" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="177"/>
-      <c r="C53" s="177"/>
-      <c r="D53" s="177"/>
-      <c r="E53" s="177"/>
-      <c r="F53" s="177"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="188"/>
+      <c r="D53" s="188"/>
+      <c r="E53" s="188"/>
+      <c r="F53" s="188"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8277,18 +8274,18 @@
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="170" t="s">
+      <c r="A54" s="208" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="171"/>
-      <c r="C54" s="167" t="s">
+      <c r="B54" s="209"/>
+      <c r="C54" s="205" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="168"/>
-      <c r="E54" s="168"/>
-      <c r="F54" s="168"/>
-      <c r="G54" s="168"/>
-      <c r="H54" s="169"/>
+      <c r="D54" s="206"/>
+      <c r="E54" s="206"/>
+      <c r="F54" s="206"/>
+      <c r="G54" s="206"/>
+      <c r="H54" s="207"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8359,14 +8356,14 @@
       <c r="Q56" s="93"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="176" t="s">
+      <c r="A57" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="177"/>
-      <c r="C57" s="177"/>
-      <c r="D57" s="177"/>
-      <c r="E57" s="177"/>
-      <c r="F57" s="177"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="188"/>
+      <c r="D57" s="188"/>
+      <c r="E57" s="188"/>
+      <c r="F57" s="188"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8383,16 +8380,16 @@
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="174" t="s">
+      <c r="A58" s="210" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="175"/>
-      <c r="C58" s="175"/>
-      <c r="D58" s="175"/>
-      <c r="E58" s="175"/>
-      <c r="F58" s="212"/>
-      <c r="G58" s="213"/>
-      <c r="H58" s="214"/>
+      <c r="B58" s="211"/>
+      <c r="C58" s="211"/>
+      <c r="D58" s="211"/>
+      <c r="E58" s="211"/>
+      <c r="F58" s="179"/>
+      <c r="G58" s="180"/>
+      <c r="H58" s="181"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8401,14 +8398,14 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="202"/>
-      <c r="B59" s="203"/>
+      <c r="A59" s="169"/>
+      <c r="B59" s="170"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="209" t="s">
+      <c r="D59" s="176" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="210"/>
-      <c r="F59" s="211"/>
+      <c r="E59" s="177"/>
+      <c r="F59" s="178"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8422,13 +8419,13 @@
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="204"/>
-      <c r="B60" s="205"/>
+      <c r="A60" s="171"/>
+      <c r="B60" s="172"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="206" t="s">
+      <c r="D60" s="173" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="207"/>
+      <c r="E60" s="174"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8440,13 +8437,13 @@
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="204"/>
-      <c r="B61" s="205"/>
+      <c r="A61" s="171"/>
+      <c r="B61" s="172"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="206" t="s">
+      <c r="D61" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="207"/>
+      <c r="E61" s="174"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8458,13 +8455,13 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="204"/>
-      <c r="B62" s="205"/>
+      <c r="A62" s="171"/>
+      <c r="B62" s="172"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="208" t="s">
+      <c r="D62" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="207"/>
+      <c r="E62" s="174"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8483,11 +8480,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="200" t="s">
+      <c r="E63" s="167" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="200"/>
-      <c r="G63" s="201"/>
+      <c r="F63" s="167"/>
+      <c r="G63" s="168"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8497,10 +8494,10 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="198" t="s">
+      <c r="A64" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="199"/>
+      <c r="B64" s="162"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -8574,6 +8571,33 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
@@ -8590,33 +8614,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="F58:H58"/>
     <mergeCell ref="C42:H42"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="42" priority="371" operator="equal">
@@ -9107,7 +9104,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A29" sqref="A5:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -9679,6 +9676,77 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </n8bc46b862004554b29f25437dcecdb2>
+    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
+    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
+    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b348aa9236b94ac88332be997039b018>
+    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
+      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
+      <Description>QWPW5C3C64YX-694079015-91</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -9899,77 +9967,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </n8bc46b862004554b29f25437dcecdb2>
-    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
-    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
-    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b348aa9236b94ac88332be997039b018>
-    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
-      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
-      <Description>QWPW5C3C64YX-694079015-91</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
@@ -9979,6 +9976,32 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9996,30 +10019,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Raised the font size of the comments in checklist to 12
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082255DB-1BF0-4B82-8660-CB66193C26F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D19F7D-AEC9-43AE-9040-27A2B4FC4180}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -3277,7 +3277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -3869,6 +3869,9 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="29" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -5221,7 +5224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AF9770-A07B-4681-91C3-E6CA1B6C7937}">
   <dimension ref="A1:IR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -6778,8 +6781,8 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7051,7 +7054,7 @@
       <c r="D13" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E13"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="88">
         <f>IF(D13="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7082,7 +7085,7 @@
       <c r="D14" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E14"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="88">
         <f>IF(D14="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7113,7 +7116,7 @@
       <c r="D15" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E15"/>
+      <c r="E15" s="65"/>
       <c r="F15" s="88">
         <f t="shared" ref="F15:F26" si="1">IF(D15="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7144,7 +7147,7 @@
       <c r="D16" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E16"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7175,7 +7178,7 @@
       <c r="D17" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E17"/>
+      <c r="E17" s="65"/>
       <c r="F17" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7206,7 +7209,7 @@
       <c r="D18" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E18"/>
+      <c r="E18" s="65"/>
       <c r="F18" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7237,7 +7240,7 @@
       <c r="D19" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E19"/>
+      <c r="E19" s="65"/>
       <c r="F19" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7270,7 +7273,7 @@
       <c r="D20" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E20"/>
+      <c r="E20" s="65"/>
       <c r="F20" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7303,7 +7306,7 @@
       <c r="D21" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E21"/>
+      <c r="E21" s="65"/>
       <c r="F21" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7336,7 +7339,7 @@
       <c r="D22" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E22"/>
+      <c r="E22" s="65"/>
       <c r="F22" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7369,7 +7372,7 @@
       <c r="D23" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E23"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7400,7 +7403,7 @@
       <c r="D24" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E24"/>
+      <c r="E24" s="65"/>
       <c r="F24" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7433,7 +7436,7 @@
       <c r="D25" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E25"/>
+      <c r="E25" s="65"/>
       <c r="F25" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7464,7 +7467,7 @@
       <c r="D26" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E26"/>
+      <c r="E26" s="65"/>
       <c r="F26" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7539,7 +7542,7 @@
       <c r="D29" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E29"/>
+      <c r="E29" s="65"/>
       <c r="F29" s="88">
         <f t="shared" ref="F29:F40" si="2">IF(D29="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7570,7 +7573,7 @@
       <c r="D30" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E30"/>
+      <c r="E30" s="65"/>
       <c r="F30" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7601,7 +7604,7 @@
       <c r="D31" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E31"/>
+      <c r="E31" s="65"/>
       <c r="F31" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7632,7 +7635,7 @@
       <c r="D32" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E32"/>
+      <c r="E32" s="65"/>
       <c r="F32" s="88"/>
       <c r="G32" s="89"/>
       <c r="H32" s="90">
@@ -7660,7 +7663,7 @@
       <c r="D33" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E33"/>
+      <c r="E33" s="65"/>
       <c r="F33" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7691,7 +7694,7 @@
       <c r="D34" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E34"/>
+      <c r="E34" s="65"/>
       <c r="F34" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7722,7 +7725,7 @@
       <c r="D35" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E35"/>
+      <c r="E35" s="65"/>
       <c r="F35" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7753,7 +7756,7 @@
       <c r="D36" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E36"/>
+      <c r="E36" s="65"/>
       <c r="F36" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7784,7 +7787,7 @@
       <c r="D37" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E37"/>
+      <c r="E37" s="65"/>
       <c r="F37" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7815,7 +7818,7 @@
       <c r="D38" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E38"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7846,7 +7849,7 @@
       <c r="D39" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E39"/>
+      <c r="E39" s="65"/>
       <c r="F39" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7877,7 +7880,7 @@
       <c r="D40" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E40"/>
+      <c r="E40" s="65"/>
       <c r="F40" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7952,7 +7955,7 @@
       <c r="D43" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E43"/>
+      <c r="E43" s="65"/>
       <c r="F43" s="88">
         <f t="shared" ref="F43:F56" si="4">IF(D43="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7983,7 +7986,7 @@
       <c r="D44" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E44"/>
+      <c r="E44" s="65"/>
       <c r="F44" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8014,7 +8017,7 @@
       <c r="D45" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E45"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8045,7 +8048,7 @@
       <c r="D46" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E46"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8076,7 +8079,7 @@
       <c r="D47" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E47"/>
+      <c r="E47" s="65"/>
       <c r="F47" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8107,7 +8110,7 @@
       <c r="D48" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E48"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8138,7 +8141,7 @@
       <c r="D49" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E49"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8169,7 +8172,7 @@
       <c r="D50" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E50"/>
+      <c r="E50" s="65"/>
       <c r="F50" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8200,7 +8203,7 @@
       <c r="D51" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E51"/>
+      <c r="E51" s="65"/>
       <c r="F51" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8231,7 +8234,7 @@
       <c r="D52" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E52"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8306,7 +8309,7 @@
       <c r="D55" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E55"/>
+      <c r="E55" s="65"/>
       <c r="F55" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8337,7 +8340,7 @@
       <c r="D56" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E56"/>
+      <c r="E56" s="65"/>
       <c r="F56" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -9105,7 +9108,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A5:XFD29"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -9199,7 +9202,7 @@
     </row>
     <row r="4" spans="1:20" s="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="138"/>
-      <c r="C4" s="139"/>
+      <c r="C4" s="217"/>
       <c r="D4" s="140"/>
       <c r="E4" s="141"/>
       <c r="F4" s="142"/>

</xml_diff>

<commit_message>
Made changes to the tempate so that there is no need to make a style for the comment column
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D19F7D-AEC9-43AE-9040-27A2B4FC4180}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27462375-23DB-4259-8E6B-ADF44FD62D28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3277,7 +3277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -3706,6 +3706,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="29" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3870,8 +3873,8 @@
     <xf numFmtId="0" fontId="33" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -6781,8 +6784,8 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6807,16 +6810,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="186" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="187"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6830,13 +6833,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="167" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="166"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="190"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="191"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6848,13 +6851,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="167" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="204"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="205"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6866,12 +6869,12 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="167" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="166"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6884,13 +6887,13 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="166" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="213"/>
-      <c r="D5" s="213"/>
-      <c r="E5" s="214"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="214"/>
+      <c r="D5" s="214"/>
+      <c r="E5" s="215"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6902,13 +6905,13 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="165" t="s">
+      <c r="A6" s="166" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="165"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="164"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="165"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6920,13 +6923,13 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="165" t="s">
+      <c r="A7" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="165"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6938,13 +6941,13 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="166" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="165"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="164"/>
+      <c r="B8" s="166"/>
+      <c r="C8" s="164"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="165"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6956,16 +6959,16 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="194" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
+      <c r="B9" s="195"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6975,16 +6978,16 @@
       <c r="Q9" s="99"/>
     </row>
     <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="195" t="s">
+      <c r="A10" s="196" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="196"/>
-      <c r="C10" s="196"/>
-      <c r="D10" s="196"/>
-      <c r="E10" s="196"/>
-      <c r="F10" s="196"/>
-      <c r="G10" s="196"/>
-      <c r="H10" s="197"/>
+      <c r="B10" s="197"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="198"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6994,10 +6997,10 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="200" t="s">
+      <c r="A11" s="201" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="201"/>
+      <c r="B11" s="202"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -7007,10 +7010,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="199" t="s">
+      <c r="F11" s="200" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="199"/>
+      <c r="G11" s="200"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -7022,18 +7025,18 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="191" t="s">
+      <c r="A12" s="192" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="192"/>
-      <c r="C12" s="182" t="s">
+      <c r="B12" s="193"/>
+      <c r="C12" s="183" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="183"/>
-      <c r="F12" s="183"/>
-      <c r="G12" s="183"/>
-      <c r="H12" s="184"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="184"/>
+      <c r="H12" s="185"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -7054,7 +7057,7 @@
       <c r="D13" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="65"/>
+      <c r="E13" s="218"/>
       <c r="F13" s="88">
         <f>IF(D13="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7085,7 +7088,7 @@
       <c r="D14" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="65"/>
+      <c r="E14" s="218"/>
       <c r="F14" s="88">
         <f>IF(D14="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7116,7 +7119,7 @@
       <c r="D15" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="65"/>
+      <c r="E15" s="218"/>
       <c r="F15" s="88">
         <f t="shared" ref="F15:F26" si="1">IF(D15="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7147,7 +7150,7 @@
       <c r="D16" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="65"/>
+      <c r="E16" s="218"/>
       <c r="F16" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7178,7 +7181,7 @@
       <c r="D17" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="65"/>
+      <c r="E17" s="218"/>
       <c r="F17" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7209,7 +7212,7 @@
       <c r="D18" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="65"/>
+      <c r="E18" s="218"/>
       <c r="F18" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7240,7 +7243,7 @@
       <c r="D19" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="65"/>
+      <c r="E19" s="218"/>
       <c r="F19" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7273,7 +7276,7 @@
       <c r="D20" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="65"/>
+      <c r="E20" s="218"/>
       <c r="F20" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7306,7 +7309,7 @@
       <c r="D21" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="65"/>
+      <c r="E21" s="218"/>
       <c r="F21" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7339,7 +7342,7 @@
       <c r="D22" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="65"/>
+      <c r="E22" s="218"/>
       <c r="F22" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7372,7 +7375,7 @@
       <c r="D23" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="65"/>
+      <c r="E23" s="218"/>
       <c r="F23" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7403,7 +7406,7 @@
       <c r="D24" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="65"/>
+      <c r="E24" s="218"/>
       <c r="F24" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7436,7 +7439,7 @@
       <c r="D25" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="218"/>
       <c r="F25" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7467,7 +7470,7 @@
       <c r="D26" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="65"/>
+      <c r="E26" s="218"/>
       <c r="F26" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7486,14 +7489,14 @@
       <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="187" t="s">
+      <c r="A27" s="188" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="188"/>
-      <c r="C27" s="188"/>
-      <c r="D27" s="188"/>
-      <c r="E27" s="188"/>
-      <c r="F27" s="188"/>
+      <c r="B27" s="189"/>
+      <c r="C27" s="189"/>
+      <c r="D27" s="189"/>
+      <c r="E27" s="189"/>
+      <c r="F27" s="189"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7510,18 +7513,18 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="191" t="s">
+      <c r="A28" s="192" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="198"/>
-      <c r="C28" s="182" t="s">
+      <c r="B28" s="199"/>
+      <c r="C28" s="183" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="183"/>
-      <c r="F28" s="183"/>
-      <c r="G28" s="183"/>
-      <c r="H28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="185"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7542,7 +7545,7 @@
       <c r="D29" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="65"/>
+      <c r="E29" s="218"/>
       <c r="F29" s="88">
         <f t="shared" ref="F29:F40" si="2">IF(D29="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7573,7 +7576,7 @@
       <c r="D30" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="65"/>
+      <c r="E30" s="218"/>
       <c r="F30" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7604,7 +7607,7 @@
       <c r="D31" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="65"/>
+      <c r="E31" s="218"/>
       <c r="F31" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7635,7 +7638,7 @@
       <c r="D32" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="65"/>
+      <c r="E32" s="218"/>
       <c r="F32" s="88"/>
       <c r="G32" s="89"/>
       <c r="H32" s="90">
@@ -7663,7 +7666,7 @@
       <c r="D33" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="65"/>
+      <c r="E33" s="218"/>
       <c r="F33" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7694,7 +7697,7 @@
       <c r="D34" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="65"/>
+      <c r="E34" s="218"/>
       <c r="F34" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7725,7 +7728,7 @@
       <c r="D35" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="65"/>
+      <c r="E35" s="218"/>
       <c r="F35" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7756,7 +7759,7 @@
       <c r="D36" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="65"/>
+      <c r="E36" s="218"/>
       <c r="F36" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7787,7 +7790,7 @@
       <c r="D37" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="65"/>
+      <c r="E37" s="218"/>
       <c r="F37" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7818,7 +7821,7 @@
       <c r="D38" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="218"/>
       <c r="F38" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7849,7 +7852,7 @@
       <c r="D39" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="65"/>
+      <c r="E39" s="218"/>
       <c r="F39" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7880,7 +7883,7 @@
       <c r="D40" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="65"/>
+      <c r="E40" s="218"/>
       <c r="F40" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7899,14 +7902,14 @@
       <c r="Q40" s="93"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="187" t="s">
+      <c r="A41" s="188" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="188"/>
-      <c r="C41" s="188"/>
-      <c r="D41" s="188"/>
-      <c r="E41" s="188"/>
-      <c r="F41" s="188"/>
+      <c r="B41" s="189"/>
+      <c r="C41" s="189"/>
+      <c r="D41" s="189"/>
+      <c r="E41" s="189"/>
+      <c r="F41" s="189"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7923,18 +7926,18 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="191" t="s">
+      <c r="A42" s="192" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="198"/>
-      <c r="C42" s="182" t="s">
+      <c r="B42" s="199"/>
+      <c r="C42" s="183" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="183"/>
-      <c r="F42" s="183"/>
-      <c r="G42" s="183"/>
-      <c r="H42" s="184"/>
+      <c r="D42" s="184"/>
+      <c r="E42" s="184"/>
+      <c r="F42" s="184"/>
+      <c r="G42" s="184"/>
+      <c r="H42" s="185"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -7955,7 +7958,7 @@
       <c r="D43" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="65"/>
+      <c r="E43" s="218"/>
       <c r="F43" s="88">
         <f t="shared" ref="F43:F56" si="4">IF(D43="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7986,7 +7989,7 @@
       <c r="D44" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="65"/>
+      <c r="E44" s="218"/>
       <c r="F44" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8017,7 +8020,7 @@
       <c r="D45" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="65"/>
+      <c r="E45" s="218"/>
       <c r="F45" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8048,7 +8051,7 @@
       <c r="D46" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="65"/>
+      <c r="E46" s="218"/>
       <c r="F46" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8079,7 +8082,7 @@
       <c r="D47" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E47" s="65"/>
+      <c r="E47" s="218"/>
       <c r="F47" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8110,7 +8113,7 @@
       <c r="D48" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="65"/>
+      <c r="E48" s="218"/>
       <c r="F48" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8141,7 +8144,7 @@
       <c r="D49" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="65"/>
+      <c r="E49" s="218"/>
       <c r="F49" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8172,7 +8175,7 @@
       <c r="D50" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="65"/>
+      <c r="E50" s="218"/>
       <c r="F50" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8203,7 +8206,7 @@
       <c r="D51" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="65"/>
+      <c r="E51" s="218"/>
       <c r="F51" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8234,7 +8237,7 @@
       <c r="D52" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E52" s="65"/>
+      <c r="E52" s="218"/>
       <c r="F52" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8253,14 +8256,14 @@
       <c r="Q52" s="93"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="187" t="s">
+      <c r="A53" s="188" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="188"/>
-      <c r="C53" s="188"/>
-      <c r="D53" s="188"/>
-      <c r="E53" s="188"/>
-      <c r="F53" s="188"/>
+      <c r="B53" s="189"/>
+      <c r="C53" s="189"/>
+      <c r="D53" s="189"/>
+      <c r="E53" s="189"/>
+      <c r="F53" s="189"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8277,18 +8280,18 @@
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="208" t="s">
+      <c r="A54" s="209" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="209"/>
-      <c r="C54" s="205" t="s">
+      <c r="B54" s="210"/>
+      <c r="C54" s="206" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="206"/>
-      <c r="E54" s="206"/>
-      <c r="F54" s="206"/>
-      <c r="G54" s="206"/>
-      <c r="H54" s="207"/>
+      <c r="D54" s="207"/>
+      <c r="E54" s="207"/>
+      <c r="F54" s="207"/>
+      <c r="G54" s="207"/>
+      <c r="H54" s="208"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8309,7 +8312,7 @@
       <c r="D55" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E55" s="65"/>
+      <c r="E55" s="218"/>
       <c r="F55" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8340,7 +8343,7 @@
       <c r="D56" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="65"/>
+      <c r="E56" s="218"/>
       <c r="F56" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8359,14 +8362,14 @@
       <c r="Q56" s="93"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="187" t="s">
+      <c r="A57" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="188"/>
-      <c r="C57" s="188"/>
-      <c r="D57" s="188"/>
-      <c r="E57" s="188"/>
-      <c r="F57" s="188"/>
+      <c r="B57" s="189"/>
+      <c r="C57" s="189"/>
+      <c r="D57" s="189"/>
+      <c r="E57" s="189"/>
+      <c r="F57" s="189"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8383,16 +8386,16 @@
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="210" t="s">
+      <c r="A58" s="211" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="211"/>
-      <c r="C58" s="211"/>
-      <c r="D58" s="211"/>
-      <c r="E58" s="211"/>
-      <c r="F58" s="179"/>
-      <c r="G58" s="180"/>
-      <c r="H58" s="181"/>
+      <c r="B58" s="212"/>
+      <c r="C58" s="212"/>
+      <c r="D58" s="212"/>
+      <c r="E58" s="212"/>
+      <c r="F58" s="180"/>
+      <c r="G58" s="181"/>
+      <c r="H58" s="182"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8401,14 +8404,14 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="169"/>
-      <c r="B59" s="170"/>
+      <c r="A59" s="170"/>
+      <c r="B59" s="171"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="176" t="s">
+      <c r="D59" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="177"/>
-      <c r="F59" s="178"/>
+      <c r="E59" s="178"/>
+      <c r="F59" s="179"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8422,13 +8425,13 @@
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="171"/>
-      <c r="B60" s="172"/>
+      <c r="A60" s="172"/>
+      <c r="B60" s="173"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="173" t="s">
+      <c r="D60" s="174" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="174"/>
+      <c r="E60" s="175"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8440,13 +8443,13 @@
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="171"/>
-      <c r="B61" s="172"/>
+      <c r="A61" s="172"/>
+      <c r="B61" s="173"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="173" t="s">
+      <c r="D61" s="174" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="174"/>
+      <c r="E61" s="175"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8458,13 +8461,13 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="171"/>
-      <c r="B62" s="172"/>
+      <c r="A62" s="172"/>
+      <c r="B62" s="173"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="175" t="s">
+      <c r="D62" s="176" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="174"/>
+      <c r="E62" s="175"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8483,11 +8486,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="167" t="s">
+      <c r="E63" s="168" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="167"/>
-      <c r="G63" s="168"/>
+      <c r="F63" s="168"/>
+      <c r="G63" s="169"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8497,10 +8500,10 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="161" t="s">
+      <c r="A64" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="162"/>
+      <c r="B64" s="163"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -9126,16 +9129,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="130" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="217" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
       <c r="I1" s="128"/>
       <c r="J1" s="128"/>
       <c r="K1" s="128"/>
@@ -9147,16 +9150,16 @@
       <c r="Q1" s="129"/>
     </row>
     <row r="2" spans="1:20" s="135" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="216" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
       <c r="I2" s="131"/>
       <c r="J2" s="132"/>
       <c r="K2" s="132"/>
@@ -9202,7 +9205,7 @@
     </row>
     <row r="4" spans="1:20" s="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="138"/>
-      <c r="C4" s="217"/>
+      <c r="C4" s="161"/>
       <c r="D4" s="140"/>
       <c r="E4" s="141"/>
       <c r="F4" s="142"/>

</xml_diff>